<commit_message>
added new scripts for new offers
</commit_message>
<xml_diff>
--- a/Updates/Input data/8682-AdvancedActionListi (7).xlsx
+++ b/Updates/Input data/8682-AdvancedActionListi (7).xlsx
@@ -123,7 +123,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I85"/>
+  <dimension ref="A1:I84"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -178,11 +178,11 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>45934.90261574074</v>
+        <v>45935.92592592593</v>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6486.553387</t>
+          <t>M.15608.6487.568983</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
@@ -201,10 +201,10 @@
         </is>
       </c>
       <c r="F2" s="6" t="n">
-        <v>47.35</v>
+        <v>88.39</v>
       </c>
       <c r="G2" s="7" t="n">
-        <v>4.74</v>
+        <v>8.84</v>
       </c>
       <c r="H2" s="8" t="inlineStr">
         <is>
@@ -219,11 +219,11 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>45934.85689814815</v>
+        <v>45935.850381944445</v>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6486.472769</t>
+          <t>M.15608.6487.461322</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
@@ -242,10 +242,10 @@
         </is>
       </c>
       <c r="F3" s="6" t="n">
-        <v>36.3</v>
+        <v>29.99</v>
       </c>
       <c r="G3" s="7" t="n">
-        <v>3.63</v>
+        <v>3.0</v>
       </c>
       <c r="H3" s="8" t="inlineStr">
         <is>
@@ -260,11 +260,11 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>45934.804236111115</v>
+        <v>45935.677824074075</v>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6486.377939</t>
+          <t>M.15608.6487.95086</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
@@ -283,10 +283,10 @@
         </is>
       </c>
       <c r="F4" s="6" t="n">
-        <v>86.82</v>
+        <v>28.41</v>
       </c>
       <c r="G4" s="7" t="n">
-        <v>8.68</v>
+        <v>2.84</v>
       </c>
       <c r="H4" s="8" t="inlineStr">
         <is>
@@ -301,11 +301,11 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>45934.66096064815</v>
+        <v>45935.59841435185</v>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6486.161300</t>
+          <t>M.15608.6487.44991</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
@@ -324,14 +324,14 @@
         </is>
       </c>
       <c r="F5" s="6" t="n">
-        <v>112.07</v>
+        <v>26.83</v>
       </c>
       <c r="G5" s="7" t="n">
-        <v>11.21</v>
+        <v>2.68</v>
       </c>
       <c r="H5" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I5" s="9" t="inlineStr">
@@ -342,11 +342,11 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>45934.63767361111</v>
+        <v>45935.55547453704</v>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6486.135911</t>
+          <t>M.15608.6487.26758</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
@@ -365,10 +365,10 @@
         </is>
       </c>
       <c r="F6" s="6" t="n">
-        <v>12.63</v>
+        <v>86.82</v>
       </c>
       <c r="G6" s="7" t="n">
-        <v>1.26</v>
+        <v>8.68</v>
       </c>
       <c r="H6" s="8" t="inlineStr">
         <is>
@@ -383,11 +383,11 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>45934.596979166665</v>
+        <v>45935.541284722225</v>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6486.94009</t>
+          <t>M.15608.6487.21349</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
@@ -397,7 +397,7 @@
       </c>
       <c r="D7" s="4" t="inlineStr">
         <is>
-          <t>Sale (iOS App)</t>
+          <t>Sale (Android App)</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
@@ -406,10 +406,10 @@
         </is>
       </c>
       <c r="F7" s="6" t="n">
-        <v>29.99</v>
+        <v>39.46</v>
       </c>
       <c r="G7" s="7" t="n">
-        <v>3.0</v>
+        <v>3.95</v>
       </c>
       <c r="H7" s="8" t="inlineStr">
         <is>
@@ -424,11 +424,11 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>45934.582453703704</v>
+        <v>45935.3608912037</v>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6486.78318</t>
+          <t>M.15608.6486.1199129</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
@@ -447,10 +447,10 @@
         </is>
       </c>
       <c r="F8" s="6" t="n">
-        <v>14.21</v>
+        <v>64.72</v>
       </c>
       <c r="G8" s="7" t="n">
-        <v>1.42</v>
+        <v>6.47</v>
       </c>
       <c r="H8" s="8" t="inlineStr">
         <is>
@@ -465,11 +465,11 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>45934.545</v>
+        <v>45935.357453703706</v>
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6486.39475</t>
+          <t>M.15608.6486.1184171</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
@@ -488,14 +488,14 @@
         </is>
       </c>
       <c r="F9" s="6" t="n">
-        <v>14.21</v>
+        <v>55.14</v>
       </c>
       <c r="G9" s="7" t="n">
-        <v>1.42</v>
+        <v>5.51</v>
       </c>
       <c r="H9" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I9" s="9" t="inlineStr">
@@ -506,11 +506,11 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>45934.53135416667</v>
+        <v>45934.90261574074</v>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6486.30882</t>
+          <t>M.15608.6486.553387</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
@@ -529,14 +529,14 @@
         </is>
       </c>
       <c r="F10" s="6" t="n">
-        <v>65.59</v>
+        <v>47.35</v>
       </c>
       <c r="G10" s="7" t="n">
-        <v>6.56</v>
+        <v>4.74</v>
       </c>
       <c r="H10" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I10" s="9" t="inlineStr">
@@ -547,11 +547,11 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>45934.503125</v>
+        <v>45934.85689814815</v>
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6486.3193</t>
+          <t>M.15608.6486.472769</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
@@ -570,10 +570,10 @@
         </is>
       </c>
       <c r="F11" s="6" t="n">
-        <v>14.21</v>
+        <v>36.3</v>
       </c>
       <c r="G11" s="7" t="n">
-        <v>1.42</v>
+        <v>3.63</v>
       </c>
       <c r="H11" s="8" t="inlineStr">
         <is>
@@ -588,11 +588,11 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>45934.18512731481</v>
+        <v>45934.804236111115</v>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6485.1063730</t>
+          <t>M.15608.6486.377939</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
@@ -611,14 +611,14 @@
         </is>
       </c>
       <c r="F12" s="6" t="n">
-        <v>83.48</v>
+        <v>86.82</v>
       </c>
       <c r="G12" s="7" t="n">
-        <v>8.35</v>
+        <v>8.68</v>
       </c>
       <c r="H12" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I12" s="9" t="inlineStr">
@@ -629,11 +629,11 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>45934.05074074074</v>
+        <v>45934.66096064815</v>
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6485.784899</t>
+          <t>M.15608.6486.161300</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
@@ -652,10 +652,10 @@
         </is>
       </c>
       <c r="F13" s="6" t="n">
-        <v>14.21</v>
+        <v>112.07</v>
       </c>
       <c r="G13" s="7" t="n">
-        <v>1.42</v>
+        <v>11.21</v>
       </c>
       <c r="H13" s="8" t="inlineStr">
         <is>
@@ -670,11 +670,11 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>45934.02245370371</v>
+        <v>45934.63767361111</v>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6485.729554</t>
+          <t>M.15608.6486.135911</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
@@ -693,10 +693,10 @@
         </is>
       </c>
       <c r="F14" s="6" t="n">
-        <v>179.95</v>
+        <v>12.63</v>
       </c>
       <c r="G14" s="7" t="n">
-        <v>17.99</v>
+        <v>1.26</v>
       </c>
       <c r="H14" s="8" t="inlineStr">
         <is>
@@ -711,11 +711,11 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>45934.02226851852</v>
+        <v>45934.596979166665</v>
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6485.729758</t>
+          <t>M.15608.6486.94009</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
@@ -734,10 +734,10 @@
         </is>
       </c>
       <c r="F15" s="6" t="n">
-        <v>110.49</v>
+        <v>29.99</v>
       </c>
       <c r="G15" s="7" t="n">
-        <v>11.05</v>
+        <v>3.0</v>
       </c>
       <c r="H15" s="8" t="inlineStr">
         <is>
@@ -752,11 +752,11 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>45934.00570601852</v>
+        <v>45934.582453703704</v>
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6485.708442</t>
+          <t>M.15608.6486.78318</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
@@ -775,10 +775,10 @@
         </is>
       </c>
       <c r="F16" s="6" t="n">
-        <v>110.49</v>
+        <v>14.21</v>
       </c>
       <c r="G16" s="7" t="n">
-        <v>11.05</v>
+        <v>1.42</v>
       </c>
       <c r="H16" s="8" t="inlineStr">
         <is>
@@ -793,11 +793,11 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>45933.99395833333</v>
+        <v>45934.545</v>
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6485.672663</t>
+          <t>M.15608.6486.39475</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
@@ -816,10 +816,10 @@
         </is>
       </c>
       <c r="F17" s="6" t="n">
-        <v>71.03</v>
+        <v>14.21</v>
       </c>
       <c r="G17" s="7" t="n">
-        <v>7.1</v>
+        <v>1.42</v>
       </c>
       <c r="H17" s="8" t="inlineStr">
         <is>
@@ -834,11 +834,11 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>45933.98636574074</v>
+        <v>45934.53135416667</v>
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6485.663296</t>
+          <t>M.15608.6486.30882</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
@@ -848,7 +848,7 @@
       </c>
       <c r="D18" s="4" t="inlineStr">
         <is>
-          <t>Sale (Android App)</t>
+          <t>Sale (iOS App)</t>
         </is>
       </c>
       <c r="E18" s="5" t="inlineStr">
@@ -857,14 +857,14 @@
         </is>
       </c>
       <c r="F18" s="6" t="n">
-        <v>61.56</v>
+        <v>65.59</v>
       </c>
       <c r="G18" s="7" t="n">
-        <v>6.16</v>
+        <v>6.56</v>
       </c>
       <c r="H18" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I18" s="9" t="inlineStr">
@@ -875,11 +875,11 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>45933.88585648148</v>
+        <v>45934.503125</v>
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6485.463996</t>
+          <t>M.15608.6486.3193</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
@@ -916,11 +916,11 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>45933.81726851852</v>
+        <v>45934.18512731481</v>
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6485.350281</t>
+          <t>M.15608.6485.1063730</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
@@ -939,14 +939,14 @@
         </is>
       </c>
       <c r="F20" s="6" t="n">
-        <v>93.13</v>
+        <v>83.48</v>
       </c>
       <c r="G20" s="7" t="n">
-        <v>9.31</v>
+        <v>8.35</v>
       </c>
       <c r="H20" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I20" s="9" t="inlineStr">
@@ -957,11 +957,11 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>45933.75896990741</v>
+        <v>45934.05074074074</v>
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6485.234639</t>
+          <t>M.15608.6485.784899</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
@@ -998,11 +998,11 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>45933.75038194445</v>
+        <v>45934.02245370371</v>
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6485.224423</t>
+          <t>M.15608.6485.729554</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
@@ -1021,14 +1021,14 @@
         </is>
       </c>
       <c r="F22" s="6" t="n">
-        <v>52.16</v>
+        <v>179.95</v>
       </c>
       <c r="G22" s="7" t="n">
-        <v>5.22</v>
+        <v>17.99</v>
       </c>
       <c r="H22" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I22" s="9" t="inlineStr">
@@ -1039,11 +1039,11 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>45933.748252314814</v>
+        <v>45934.02226851852</v>
       </c>
       <c r="B23" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6485.222948</t>
+          <t>M.15608.6485.729758</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
@@ -1062,10 +1062,10 @@
         </is>
       </c>
       <c r="F23" s="6" t="n">
-        <v>26.83</v>
+        <v>110.49</v>
       </c>
       <c r="G23" s="7" t="n">
-        <v>2.68</v>
+        <v>11.05</v>
       </c>
       <c r="H23" s="8" t="inlineStr">
         <is>
@@ -1080,11 +1080,11 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>45933.60122685185</v>
+        <v>45934.00570601852</v>
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6485.53178</t>
+          <t>M.15608.6485.708442</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
@@ -1103,10 +1103,10 @@
         </is>
       </c>
       <c r="F24" s="6" t="n">
-        <v>14.21</v>
+        <v>110.49</v>
       </c>
       <c r="G24" s="7" t="n">
-        <v>1.42</v>
+        <v>11.05</v>
       </c>
       <c r="H24" s="8" t="inlineStr">
         <is>
@@ -1121,11 +1121,11 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>45933.590578703705</v>
+        <v>45933.99395833333</v>
       </c>
       <c r="B25" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6485.47628</t>
+          <t>M.15608.6485.672663</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
@@ -1144,10 +1144,10 @@
         </is>
       </c>
       <c r="F25" s="6" t="n">
-        <v>12.63</v>
+        <v>71.03</v>
       </c>
       <c r="G25" s="7" t="n">
-        <v>1.26</v>
+        <v>7.1</v>
       </c>
       <c r="H25" s="8" t="inlineStr">
         <is>
@@ -1162,11 +1162,11 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>45933.571388888886</v>
+        <v>45933.98636574074</v>
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6485.37454</t>
+          <t>M.15608.6485.663296</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
@@ -1176,7 +1176,7 @@
       </c>
       <c r="D26" s="4" t="inlineStr">
         <is>
-          <t>Sale (iOS App)</t>
+          <t>Sale (Android App)</t>
         </is>
       </c>
       <c r="E26" s="5" t="inlineStr">
@@ -1185,10 +1185,10 @@
         </is>
       </c>
       <c r="F26" s="6" t="n">
-        <v>36.3</v>
+        <v>61.56</v>
       </c>
       <c r="G26" s="7" t="n">
-        <v>3.63</v>
+        <v>6.16</v>
       </c>
       <c r="H26" s="8" t="inlineStr">
         <is>
@@ -1203,11 +1203,11 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>45933.561574074076</v>
+        <v>45933.88585648148</v>
       </c>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6485.32746</t>
+          <t>M.15608.6485.463996</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
@@ -1226,10 +1226,10 @@
         </is>
       </c>
       <c r="F27" s="6" t="n">
-        <v>110.49</v>
+        <v>14.21</v>
       </c>
       <c r="G27" s="7" t="n">
-        <v>11.05</v>
+        <v>1.42</v>
       </c>
       <c r="H27" s="8" t="inlineStr">
         <is>
@@ -1244,11 +1244,11 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>45933.543275462966</v>
+        <v>45933.81726851852</v>
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6485.23786</t>
+          <t>M.15608.6485.350281</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
@@ -1267,10 +1267,10 @@
         </is>
       </c>
       <c r="F28" s="6" t="n">
-        <v>39.46</v>
+        <v>93.13</v>
       </c>
       <c r="G28" s="7" t="n">
-        <v>3.95</v>
+        <v>9.31</v>
       </c>
       <c r="H28" s="8" t="inlineStr">
         <is>
@@ -1285,11 +1285,11 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>45933.40354166667</v>
+        <v>45933.75896990741</v>
       </c>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6484.1226209</t>
+          <t>M.15608.6485.234639</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
@@ -1308,10 +1308,10 @@
         </is>
       </c>
       <c r="F29" s="6" t="n">
-        <v>58.4</v>
+        <v>14.21</v>
       </c>
       <c r="G29" s="7" t="n">
-        <v>5.84</v>
+        <v>1.42</v>
       </c>
       <c r="H29" s="8" t="inlineStr">
         <is>
@@ -1326,11 +1326,11 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>45933.2671412037</v>
+        <v>45933.75038194445</v>
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6484.1092631</t>
+          <t>M.15608.6485.224423</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
@@ -1349,14 +1349,14 @@
         </is>
       </c>
       <c r="F30" s="6" t="n">
-        <v>64.72</v>
+        <v>52.16</v>
       </c>
       <c r="G30" s="7" t="n">
-        <v>6.47</v>
+        <v>5.22</v>
       </c>
       <c r="H30" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I30" s="9" t="inlineStr">
@@ -1367,11 +1367,11 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>45932.96487268519</v>
+        <v>45933.748252314814</v>
       </c>
       <c r="B31" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6484.540290</t>
+          <t>M.15608.6485.222948</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
@@ -1390,10 +1390,10 @@
         </is>
       </c>
       <c r="F31" s="6" t="n">
-        <v>110.49</v>
+        <v>26.83</v>
       </c>
       <c r="G31" s="7" t="n">
-        <v>11.05</v>
+        <v>2.68</v>
       </c>
       <c r="H31" s="8" t="inlineStr">
         <is>
@@ -1408,11 +1408,11 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>45932.92831018518</v>
+        <v>45933.60122685185</v>
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6484.452004</t>
+          <t>M.15608.6485.53178</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
@@ -1431,14 +1431,14 @@
         </is>
       </c>
       <c r="F32" s="6" t="n">
-        <v>29.63</v>
+        <v>14.21</v>
       </c>
       <c r="G32" s="7" t="n">
-        <v>2.96</v>
+        <v>1.42</v>
       </c>
       <c r="H32" s="8" t="inlineStr">
         <is>
-          <t>D35</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I32" s="9" t="inlineStr">
@@ -1449,11 +1449,11 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>45932.81166666667</v>
+        <v>45933.590578703705</v>
       </c>
       <c r="B33" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6484.256134</t>
+          <t>M.15608.6485.47628</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
@@ -1472,14 +1472,14 @@
         </is>
       </c>
       <c r="F33" s="6" t="n">
-        <v>122.24</v>
+        <v>12.63</v>
       </c>
       <c r="G33" s="7" t="n">
-        <v>12.22</v>
+        <v>1.26</v>
       </c>
       <c r="H33" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I33" s="9" t="inlineStr">
@@ -1490,11 +1490,11 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>45932.68298611111</v>
+        <v>45933.571388888886</v>
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6484.104465</t>
+          <t>M.15608.6485.37454</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr">
@@ -1531,11 +1531,11 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>45932.6625462963</v>
+        <v>45933.561574074076</v>
       </c>
       <c r="B35" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6484.88865</t>
+          <t>M.15608.6485.32746</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr">
@@ -1554,10 +1554,10 @@
         </is>
       </c>
       <c r="F35" s="6" t="n">
-        <v>45.78</v>
+        <v>110.49</v>
       </c>
       <c r="G35" s="7" t="n">
-        <v>4.58</v>
+        <v>11.05</v>
       </c>
       <c r="H35" s="8" t="inlineStr">
         <is>
@@ -1572,11 +1572,11 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>45932.636030092595</v>
+        <v>45933.543275462966</v>
       </c>
       <c r="B36" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6484.70793</t>
+          <t>M.15608.6485.23786</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr">
@@ -1595,10 +1595,10 @@
         </is>
       </c>
       <c r="F36" s="6" t="n">
-        <v>45.78</v>
+        <v>39.46</v>
       </c>
       <c r="G36" s="7" t="n">
-        <v>4.58</v>
+        <v>3.95</v>
       </c>
       <c r="H36" s="8" t="inlineStr">
         <is>
@@ -1613,11 +1613,11 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>45932.540613425925</v>
+        <v>45933.40354166667</v>
       </c>
       <c r="B37" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6484.22125</t>
+          <t>M.15608.6484.1226209</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
@@ -1636,10 +1636,10 @@
         </is>
       </c>
       <c r="F37" s="6" t="n">
-        <v>52.09</v>
+        <v>58.4</v>
       </c>
       <c r="G37" s="7" t="n">
-        <v>5.21</v>
+        <v>5.84</v>
       </c>
       <c r="H37" s="8" t="inlineStr">
         <is>
@@ -1654,11 +1654,11 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>45932.51752314815</v>
+        <v>45933.2671412037</v>
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6484.10213</t>
+          <t>M.15608.6484.1092631</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
@@ -1677,10 +1677,10 @@
         </is>
       </c>
       <c r="F38" s="6" t="n">
-        <v>28.41</v>
+        <v>64.72</v>
       </c>
       <c r="G38" s="7" t="n">
-        <v>2.84</v>
+        <v>6.47</v>
       </c>
       <c r="H38" s="8" t="inlineStr">
         <is>
@@ -1695,11 +1695,11 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>45932.408530092594</v>
+        <v>45932.96487268519</v>
       </c>
       <c r="B39" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6483.1228977</t>
+          <t>M.15608.6484.540290</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
@@ -1718,14 +1718,14 @@
         </is>
       </c>
       <c r="F39" s="6" t="n">
-        <v>61.1</v>
+        <v>110.49</v>
       </c>
       <c r="G39" s="7" t="n">
-        <v>6.11</v>
+        <v>11.05</v>
       </c>
       <c r="H39" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I39" s="9" t="inlineStr">
@@ -1736,11 +1736,11 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>45932.39805555555</v>
+        <v>45932.92831018518</v>
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6483.1212476</t>
+          <t>M.15608.6484.452004</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
@@ -1759,14 +1759,14 @@
         </is>
       </c>
       <c r="F40" s="6" t="n">
-        <v>17.36</v>
+        <v>29.63</v>
       </c>
       <c r="G40" s="7" t="n">
-        <v>1.74</v>
+        <v>2.96</v>
       </c>
       <c r="H40" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>D35</t>
         </is>
       </c>
       <c r="I40" s="9" t="inlineStr">
@@ -1777,11 +1777,11 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>45932.14304398148</v>
+        <v>45932.81166666667</v>
       </c>
       <c r="B41" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6483.967351</t>
+          <t>M.15608.6484.256134</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
@@ -1800,10 +1800,10 @@
         </is>
       </c>
       <c r="F41" s="6" t="n">
-        <v>59.49</v>
+        <v>122.24</v>
       </c>
       <c r="G41" s="7" t="n">
-        <v>5.95</v>
+        <v>12.22</v>
       </c>
       <c r="H41" s="8" t="inlineStr">
         <is>
@@ -1818,11 +1818,11 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>45931.955972222226</v>
+        <v>45932.68298611111</v>
       </c>
       <c r="B42" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6483.626399</t>
+          <t>M.15608.6484.104465</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr">
@@ -1841,10 +1841,10 @@
         </is>
       </c>
       <c r="F42" s="6" t="n">
-        <v>14.21</v>
+        <v>36.3</v>
       </c>
       <c r="G42" s="7" t="n">
-        <v>1.42</v>
+        <v>3.63</v>
       </c>
       <c r="H42" s="8" t="inlineStr">
         <is>
@@ -1859,11 +1859,11 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>45931.89545138889</v>
+        <v>45932.6625462963</v>
       </c>
       <c r="B43" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6483.512475</t>
+          <t>M.15608.6484.88865</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
@@ -1882,10 +1882,10 @@
         </is>
       </c>
       <c r="F43" s="6" t="n">
-        <v>55.25</v>
+        <v>45.78</v>
       </c>
       <c r="G43" s="7" t="n">
-        <v>5.52</v>
+        <v>4.58</v>
       </c>
       <c r="H43" s="8" t="inlineStr">
         <is>
@@ -1900,11 +1900,11 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>45931.81099537037</v>
+        <v>45932.636030092595</v>
       </c>
       <c r="B44" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6483.352117</t>
+          <t>M.15608.6484.70793</t>
         </is>
       </c>
       <c r="C44" s="3" t="inlineStr">
@@ -1923,10 +1923,10 @@
         </is>
       </c>
       <c r="F44" s="6" t="n">
-        <v>28.41</v>
+        <v>45.78</v>
       </c>
       <c r="G44" s="7" t="n">
-        <v>2.84</v>
+        <v>4.58</v>
       </c>
       <c r="H44" s="8" t="inlineStr">
         <is>
@@ -1941,11 +1941,11 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>45931.80322916667</v>
+        <v>45932.540613425925</v>
       </c>
       <c r="B45" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6483.339235</t>
+          <t>M.15608.6484.22125</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
@@ -1964,10 +1964,10 @@
         </is>
       </c>
       <c r="F45" s="6" t="n">
-        <v>28.41</v>
+        <v>52.09</v>
       </c>
       <c r="G45" s="7" t="n">
-        <v>2.84</v>
+        <v>5.21</v>
       </c>
       <c r="H45" s="8" t="inlineStr">
         <is>
@@ -1982,11 +1982,11 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>45931.73730324074</v>
+        <v>45932.51752314815</v>
       </c>
       <c r="B46" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6483.203773</t>
+          <t>M.15608.6484.10213</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
@@ -2023,11 +2023,11 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>45931.677453703705</v>
+        <v>45932.408530092594</v>
       </c>
       <c r="B47" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6483.112339</t>
+          <t>M.15608.6483.1228977</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
@@ -2046,14 +2046,14 @@
         </is>
       </c>
       <c r="F47" s="6" t="n">
-        <v>14.21</v>
+        <v>61.1</v>
       </c>
       <c r="G47" s="7" t="n">
-        <v>1.42</v>
+        <v>6.11</v>
       </c>
       <c r="H47" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I47" s="9" t="inlineStr">
@@ -2064,11 +2064,11 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>45931.67476851852</v>
+        <v>45932.39805555555</v>
       </c>
       <c r="B48" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6483.110261</t>
+          <t>M.15608.6483.1212476</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr">
@@ -2087,10 +2087,10 @@
         </is>
       </c>
       <c r="F48" s="6" t="n">
-        <v>14.21</v>
+        <v>17.36</v>
       </c>
       <c r="G48" s="7" t="n">
-        <v>1.42</v>
+        <v>1.74</v>
       </c>
       <c r="H48" s="8" t="inlineStr">
         <is>
@@ -2105,11 +2105,11 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>45931.63186342592</v>
+        <v>45932.14304398148</v>
       </c>
       <c r="B49" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6483.79557</t>
+          <t>M.15608.6483.967351</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr">
@@ -2128,14 +2128,14 @@
         </is>
       </c>
       <c r="F49" s="6" t="n">
-        <v>44.2</v>
+        <v>59.49</v>
       </c>
       <c r="G49" s="7" t="n">
-        <v>4.42</v>
+        <v>5.95</v>
       </c>
       <c r="H49" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I49" s="9" t="inlineStr">
@@ -2146,11 +2146,11 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>45931.50315972222</v>
+        <v>45931.955972222226</v>
       </c>
       <c r="B50" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6483.1918</t>
+          <t>M.15608.6483.626399</t>
         </is>
       </c>
       <c r="C50" s="3" t="inlineStr">
@@ -2169,10 +2169,10 @@
         </is>
       </c>
       <c r="F50" s="6" t="n">
-        <v>55.25</v>
+        <v>14.21</v>
       </c>
       <c r="G50" s="7" t="n">
-        <v>5.52</v>
+        <v>1.42</v>
       </c>
       <c r="H50" s="8" t="inlineStr">
         <is>
@@ -2187,11 +2187,11 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>45931.48385416667</v>
+        <v>45931.89545138889</v>
       </c>
       <c r="B51" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6482.1391354</t>
+          <t>M.15608.6483.512475</t>
         </is>
       </c>
       <c r="C51" s="3" t="inlineStr">
@@ -2210,10 +2210,10 @@
         </is>
       </c>
       <c r="F51" s="6" t="n">
-        <v>44.2</v>
+        <v>55.25</v>
       </c>
       <c r="G51" s="7" t="n">
-        <v>4.42</v>
+        <v>5.52</v>
       </c>
       <c r="H51" s="8" t="inlineStr">
         <is>
@@ -2228,11 +2228,11 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>45931.46702546296</v>
+        <v>45931.81099537037</v>
       </c>
       <c r="B52" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6482.1375918</t>
+          <t>M.15608.6483.352117</t>
         </is>
       </c>
       <c r="C52" s="3" t="inlineStr">
@@ -2251,10 +2251,10 @@
         </is>
       </c>
       <c r="F52" s="6" t="n">
-        <v>14.21</v>
+        <v>28.41</v>
       </c>
       <c r="G52" s="7" t="n">
-        <v>1.42</v>
+        <v>2.84</v>
       </c>
       <c r="H52" s="8" t="inlineStr">
         <is>
@@ -2269,11 +2269,11 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>45931.36540509259</v>
+        <v>45931.80322916667</v>
       </c>
       <c r="B53" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6482.1256968</t>
+          <t>M.15608.6483.339235</t>
         </is>
       </c>
       <c r="C53" s="3" t="inlineStr">
@@ -2292,10 +2292,10 @@
         </is>
       </c>
       <c r="F53" s="6" t="n">
-        <v>39.46</v>
+        <v>28.41</v>
       </c>
       <c r="G53" s="7" t="n">
-        <v>3.95</v>
+        <v>2.84</v>
       </c>
       <c r="H53" s="8" t="inlineStr">
         <is>
@@ -2310,11 +2310,11 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>45931.341099537036</v>
+        <v>45931.73730324074</v>
       </c>
       <c r="B54" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6482.1239968</t>
+          <t>M.15608.6483.203773</t>
         </is>
       </c>
       <c r="C54" s="3" t="inlineStr">
@@ -2333,10 +2333,10 @@
         </is>
       </c>
       <c r="F54" s="6" t="n">
-        <v>41.04</v>
+        <v>28.41</v>
       </c>
       <c r="G54" s="7" t="n">
-        <v>4.1</v>
+        <v>2.84</v>
       </c>
       <c r="H54" s="8" t="inlineStr">
         <is>
@@ -2351,11 +2351,11 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>45931.31701388889</v>
+        <v>45931.677453703705</v>
       </c>
       <c r="B55" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6482.1209917</t>
+          <t>M.15608.6483.112339</t>
         </is>
       </c>
       <c r="C55" s="3" t="inlineStr">
@@ -2374,10 +2374,10 @@
         </is>
       </c>
       <c r="F55" s="6" t="n">
-        <v>110.49</v>
+        <v>14.21</v>
       </c>
       <c r="G55" s="7" t="n">
-        <v>11.05</v>
+        <v>1.42</v>
       </c>
       <c r="H55" s="8" t="inlineStr">
         <is>
@@ -2392,11 +2392,11 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>45931.30383101852</v>
+        <v>45931.67476851852</v>
       </c>
       <c r="B56" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6482.1198944</t>
+          <t>M.15608.6483.110261</t>
         </is>
       </c>
       <c r="C56" s="3" t="inlineStr">
@@ -2415,14 +2415,14 @@
         </is>
       </c>
       <c r="F56" s="6" t="n">
-        <v>17.89</v>
+        <v>14.21</v>
       </c>
       <c r="G56" s="7" t="n">
-        <v>1.79</v>
+        <v>1.42</v>
       </c>
       <c r="H56" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I56" s="9" t="inlineStr">
@@ -2433,11 +2433,11 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>45931.25746527778</v>
+        <v>45931.63186342592</v>
       </c>
       <c r="B57" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6482.1145343</t>
+          <t>M.15608.6483.79557</t>
         </is>
       </c>
       <c r="C57" s="3" t="inlineStr">
@@ -2456,14 +2456,14 @@
         </is>
       </c>
       <c r="F57" s="6" t="n">
-        <v>146.1</v>
+        <v>44.2</v>
       </c>
       <c r="G57" s="7" t="n">
-        <v>14.61</v>
+        <v>4.42</v>
       </c>
       <c r="H57" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I57" s="9" t="inlineStr">
@@ -2474,11 +2474,11 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>45930.92653935185</v>
+        <v>45931.50315972222</v>
       </c>
       <c r="B58" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6482.562919</t>
+          <t>M.15608.6483.1918</t>
         </is>
       </c>
       <c r="C58" s="3" t="inlineStr">
@@ -2497,7 +2497,7 @@
         </is>
       </c>
       <c r="F58" s="6" t="n">
-        <v>55.24</v>
+        <v>55.25</v>
       </c>
       <c r="G58" s="7" t="n">
         <v>5.52</v>
@@ -2515,11 +2515,11 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>45930.74658564815</v>
+        <v>45931.48385416667</v>
       </c>
       <c r="B59" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6482.211929</t>
+          <t>M.15608.6482.1391354</t>
         </is>
       </c>
       <c r="C59" s="3" t="inlineStr">
@@ -2529,7 +2529,7 @@
       </c>
       <c r="D59" s="4" t="inlineStr">
         <is>
-          <t>Sale (Android App)</t>
+          <t>Sale (iOS App)</t>
         </is>
       </c>
       <c r="E59" s="5" t="inlineStr">
@@ -2538,10 +2538,10 @@
         </is>
       </c>
       <c r="F59" s="6" t="n">
-        <v>51.83</v>
+        <v>44.2</v>
       </c>
       <c r="G59" s="7" t="n">
-        <v>5.18</v>
+        <v>4.42</v>
       </c>
       <c r="H59" s="8" t="inlineStr">
         <is>
@@ -2556,11 +2556,11 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>45930.454872685186</v>
+        <v>45931.46702546296</v>
       </c>
       <c r="B60" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6481.1355187</t>
+          <t>M.15608.6482.1375918</t>
         </is>
       </c>
       <c r="C60" s="3" t="inlineStr">
@@ -2579,14 +2579,14 @@
         </is>
       </c>
       <c r="F60" s="6" t="n">
-        <v>265.32</v>
+        <v>14.21</v>
       </c>
       <c r="G60" s="7" t="n">
-        <v>26.53</v>
+        <v>1.42</v>
       </c>
       <c r="H60" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I60" s="9" t="inlineStr">
@@ -2597,11 +2597,11 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>45930.279074074075</v>
+        <v>45931.36540509259</v>
       </c>
       <c r="B61" s="2" t="inlineStr">
         <is>
-          <t>15608.6481.1176060</t>
+          <t>M.15608.6482.1256968</t>
         </is>
       </c>
       <c r="C61" s="3" t="inlineStr">
@@ -2611,7 +2611,7 @@
       </c>
       <c r="D61" s="4" t="inlineStr">
         <is>
-          <t>Sale</t>
+          <t>Sale (iOS App)</t>
         </is>
       </c>
       <c r="E61" s="5" t="inlineStr">
@@ -2620,14 +2620,14 @@
         </is>
       </c>
       <c r="F61" s="6" t="n">
-        <v>36.3</v>
+        <v>39.46</v>
       </c>
       <c r="G61" s="7" t="n">
-        <v>3.63</v>
+        <v>3.95</v>
       </c>
       <c r="H61" s="8" t="inlineStr">
         <is>
-          <t>D26</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I61" s="9" t="inlineStr">
@@ -2638,11 +2638,11 @@
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>45930.22298611111</v>
+        <v>45931.341099537036</v>
       </c>
       <c r="B62" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6481.1099989</t>
+          <t>M.15608.6482.1239968</t>
         </is>
       </c>
       <c r="C62" s="3" t="inlineStr">
@@ -2661,10 +2661,10 @@
         </is>
       </c>
       <c r="F62" s="6" t="n">
-        <v>25.25</v>
+        <v>41.04</v>
       </c>
       <c r="G62" s="7" t="n">
-        <v>2.53</v>
+        <v>4.1</v>
       </c>
       <c r="H62" s="8" t="inlineStr">
         <is>
@@ -2679,11 +2679,11 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>45930.125601851854</v>
+        <v>45931.31701388889</v>
       </c>
       <c r="B63" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6481.957577</t>
+          <t>M.15608.6482.1209917</t>
         </is>
       </c>
       <c r="C63" s="3" t="inlineStr">
@@ -2693,7 +2693,7 @@
       </c>
       <c r="D63" s="4" t="inlineStr">
         <is>
-          <t>Sale (Android App)</t>
+          <t>Sale (iOS App)</t>
         </is>
       </c>
       <c r="E63" s="5" t="inlineStr">
@@ -2702,14 +2702,14 @@
         </is>
       </c>
       <c r="F63" s="6" t="n">
-        <v>28.02</v>
+        <v>110.49</v>
       </c>
       <c r="G63" s="7" t="n">
-        <v>2.8</v>
+        <v>11.05</v>
       </c>
       <c r="H63" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I63" s="9" t="inlineStr">
@@ -2720,11 +2720,11 @@
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>45930.09780092593</v>
+        <v>45931.30383101852</v>
       </c>
       <c r="B64" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6481.892957</t>
+          <t>M.15608.6482.1198944</t>
         </is>
       </c>
       <c r="C64" s="3" t="inlineStr">
@@ -2743,10 +2743,10 @@
         </is>
       </c>
       <c r="F64" s="6" t="n">
-        <v>58.11</v>
+        <v>17.89</v>
       </c>
       <c r="G64" s="7" t="n">
-        <v>5.81</v>
+        <v>1.79</v>
       </c>
       <c r="H64" s="8" t="inlineStr">
         <is>
@@ -2761,11 +2761,11 @@
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>45930.095509259256</v>
+        <v>45931.25746527778</v>
       </c>
       <c r="B65" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6481.891385</t>
+          <t>M.15608.6482.1145343</t>
         </is>
       </c>
       <c r="C65" s="3" t="inlineStr">
@@ -2784,10 +2784,10 @@
         </is>
       </c>
       <c r="F65" s="6" t="n">
-        <v>104.34</v>
+        <v>146.1</v>
       </c>
       <c r="G65" s="7" t="n">
-        <v>10.43</v>
+        <v>14.61</v>
       </c>
       <c r="H65" s="8" t="inlineStr">
         <is>
@@ -2802,11 +2802,11 @@
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>45930.083402777775</v>
+        <v>45930.92653935185</v>
       </c>
       <c r="B66" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6481.874839</t>
+          <t>M.15608.6482.562919</t>
         </is>
       </c>
       <c r="C66" s="3" t="inlineStr">
@@ -2825,10 +2825,10 @@
         </is>
       </c>
       <c r="F66" s="6" t="n">
-        <v>110.48</v>
+        <v>55.24</v>
       </c>
       <c r="G66" s="7" t="n">
-        <v>11.05</v>
+        <v>5.52</v>
       </c>
       <c r="H66" s="8" t="inlineStr">
         <is>
@@ -2843,11 +2843,11 @@
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>45930.03109953704</v>
+        <v>45930.74658564815</v>
       </c>
       <c r="B67" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6481.754754</t>
+          <t>M.15608.6482.211929</t>
         </is>
       </c>
       <c r="C67" s="3" t="inlineStr">
@@ -2857,7 +2857,7 @@
       </c>
       <c r="D67" s="4" t="inlineStr">
         <is>
-          <t>Sale (iOS App)</t>
+          <t>Sale (Android App)</t>
         </is>
       </c>
       <c r="E67" s="5" t="inlineStr">
@@ -2866,10 +2866,10 @@
         </is>
       </c>
       <c r="F67" s="6" t="n">
-        <v>110.48</v>
+        <v>51.83</v>
       </c>
       <c r="G67" s="7" t="n">
-        <v>11.05</v>
+        <v>5.18</v>
       </c>
       <c r="H67" s="8" t="inlineStr">
         <is>
@@ -2884,11 +2884,11 @@
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>45929.79486111111</v>
+        <v>45930.454872685186</v>
       </c>
       <c r="B68" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6481.339089</t>
+          <t>M.15608.6481.1355187</t>
         </is>
       </c>
       <c r="C68" s="3" t="inlineStr">
@@ -2907,14 +2907,14 @@
         </is>
       </c>
       <c r="F68" s="6" t="n">
-        <v>36.3</v>
+        <v>265.32</v>
       </c>
       <c r="G68" s="7" t="n">
-        <v>3.63</v>
+        <v>26.53</v>
       </c>
       <c r="H68" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I68" s="9" t="inlineStr">
@@ -2925,11 +2925,11 @@
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>45929.791863425926</v>
+        <v>45930.279074074075</v>
       </c>
       <c r="B69" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6481.328255</t>
+          <t>15608.6481.1176060</t>
         </is>
       </c>
       <c r="C69" s="3" t="inlineStr">
@@ -2939,7 +2939,7 @@
       </c>
       <c r="D69" s="4" t="inlineStr">
         <is>
-          <t>Sale (iOS App)</t>
+          <t>Sale</t>
         </is>
       </c>
       <c r="E69" s="5" t="inlineStr">
@@ -2948,14 +2948,14 @@
         </is>
       </c>
       <c r="F69" s="6" t="n">
-        <v>110.48</v>
+        <v>36.3</v>
       </c>
       <c r="G69" s="7" t="n">
-        <v>11.05</v>
+        <v>3.63</v>
       </c>
       <c r="H69" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>D26</t>
         </is>
       </c>
       <c r="I69" s="9" t="inlineStr">
@@ -2966,11 +2966,11 @@
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>45929.6397337963</v>
+        <v>45930.22298611111</v>
       </c>
       <c r="B70" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6481.81653</t>
+          <t>M.15608.6481.1099989</t>
         </is>
       </c>
       <c r="C70" s="3" t="inlineStr">
@@ -2989,14 +2989,14 @@
         </is>
       </c>
       <c r="F70" s="6" t="n">
-        <v>137.13</v>
+        <v>25.25</v>
       </c>
       <c r="G70" s="7" t="n">
-        <v>13.71</v>
+        <v>2.53</v>
       </c>
       <c r="H70" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I70" s="9" t="inlineStr">
@@ -3007,11 +3007,11 @@
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>45929.61986111111</v>
+        <v>45930.125601851854</v>
       </c>
       <c r="B71" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6481.70161</t>
+          <t>M.15608.6481.957577</t>
         </is>
       </c>
       <c r="C71" s="3" t="inlineStr">
@@ -3021,7 +3021,7 @@
       </c>
       <c r="D71" s="4" t="inlineStr">
         <is>
-          <t>Sale (iOS App)</t>
+          <t>Sale (Android App)</t>
         </is>
       </c>
       <c r="E71" s="5" t="inlineStr">
@@ -3030,14 +3030,14 @@
         </is>
       </c>
       <c r="F71" s="6" t="n">
-        <v>52.08</v>
+        <v>28.02</v>
       </c>
       <c r="G71" s="7" t="n">
-        <v>5.21</v>
+        <v>2.8</v>
       </c>
       <c r="H71" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I71" s="9" t="inlineStr">
@@ -3048,11 +3048,11 @@
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>45929.51945601852</v>
+        <v>45930.09780092593</v>
       </c>
       <c r="B72" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6481.12232</t>
+          <t>M.15608.6481.892957</t>
         </is>
       </c>
       <c r="C72" s="3" t="inlineStr">
@@ -3071,14 +3071,14 @@
         </is>
       </c>
       <c r="F72" s="6" t="n">
-        <v>110.48</v>
+        <v>58.11</v>
       </c>
       <c r="G72" s="7" t="n">
-        <v>11.05</v>
+        <v>5.81</v>
       </c>
       <c r="H72" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I72" s="9" t="inlineStr">
@@ -3089,11 +3089,11 @@
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>45929.51195601852</v>
+        <v>45930.095509259256</v>
       </c>
       <c r="B73" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6481.9150</t>
+          <t>M.15608.6481.891385</t>
         </is>
       </c>
       <c r="C73" s="3" t="inlineStr">
@@ -3112,14 +3112,14 @@
         </is>
       </c>
       <c r="F73" s="6" t="n">
-        <v>14.2</v>
+        <v>104.34</v>
       </c>
       <c r="G73" s="7" t="n">
-        <v>1.42</v>
+        <v>10.43</v>
       </c>
       <c r="H73" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I73" s="9" t="inlineStr">
@@ -3130,11 +3130,11 @@
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>45929.06377314815</v>
+        <v>45930.083402777775</v>
       </c>
       <c r="B74" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6480.786055</t>
+          <t>M.15608.6481.874839</t>
         </is>
       </c>
       <c r="C74" s="3" t="inlineStr">
@@ -3153,14 +3153,14 @@
         </is>
       </c>
       <c r="F74" s="6" t="n">
-        <v>52.15</v>
+        <v>110.48</v>
       </c>
       <c r="G74" s="7" t="n">
-        <v>5.22</v>
+        <v>11.05</v>
       </c>
       <c r="H74" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I74" s="9" t="inlineStr">
@@ -3171,11 +3171,11 @@
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>45929.05862268519</v>
+        <v>45930.03109953704</v>
       </c>
       <c r="B75" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6480.778925</t>
+          <t>M.15608.6481.754754</t>
         </is>
       </c>
       <c r="C75" s="3" t="inlineStr">
@@ -3194,10 +3194,10 @@
         </is>
       </c>
       <c r="F75" s="6" t="n">
-        <v>56.82</v>
+        <v>110.48</v>
       </c>
       <c r="G75" s="7" t="n">
-        <v>5.68</v>
+        <v>11.05</v>
       </c>
       <c r="H75" s="8" t="inlineStr">
         <is>
@@ -3212,11 +3212,11 @@
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>45928.986238425925</v>
+        <v>45929.79486111111</v>
       </c>
       <c r="B76" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6480.633048</t>
+          <t>M.15608.6481.339089</t>
         </is>
       </c>
       <c r="C76" s="3" t="inlineStr">
@@ -3235,14 +3235,14 @@
         </is>
       </c>
       <c r="F76" s="6" t="n">
-        <v>20.52</v>
+        <v>36.3</v>
       </c>
       <c r="G76" s="7" t="n">
-        <v>2.05</v>
+        <v>3.63</v>
       </c>
       <c r="H76" s="8" t="inlineStr">
         <is>
-          <t>D26</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I76" s="9" t="inlineStr">
@@ -3253,11 +3253,11 @@
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>45928.82664351852</v>
+        <v>45929.791863425926</v>
       </c>
       <c r="B77" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6480.326985</t>
+          <t>M.15608.6481.328255</t>
         </is>
       </c>
       <c r="C77" s="3" t="inlineStr">
@@ -3276,10 +3276,10 @@
         </is>
       </c>
       <c r="F77" s="6" t="n">
-        <v>28.41</v>
+        <v>110.48</v>
       </c>
       <c r="G77" s="7" t="n">
-        <v>2.84</v>
+        <v>11.05</v>
       </c>
       <c r="H77" s="8" t="inlineStr">
         <is>
@@ -3294,11 +3294,11 @@
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>45928.68114583333</v>
+        <v>45929.6397337963</v>
       </c>
       <c r="B78" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6480.112902</t>
+          <t>M.15608.6481.81653</t>
         </is>
       </c>
       <c r="C78" s="3" t="inlineStr">
@@ -3317,14 +3317,14 @@
         </is>
       </c>
       <c r="F78" s="6" t="n">
-        <v>14.2</v>
+        <v>137.13</v>
       </c>
       <c r="G78" s="7" t="n">
-        <v>1.42</v>
+        <v>13.71</v>
       </c>
       <c r="H78" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I78" s="9" t="inlineStr">
@@ -3335,11 +3335,11 @@
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>45928.58710648148</v>
+        <v>45929.61986111111</v>
       </c>
       <c r="B79" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6480.37859</t>
+          <t>M.15608.6481.70161</t>
         </is>
       </c>
       <c r="C79" s="3" t="inlineStr">
@@ -3358,14 +3358,14 @@
         </is>
       </c>
       <c r="F79" s="6" t="n">
-        <v>87.93</v>
+        <v>52.08</v>
       </c>
       <c r="G79" s="7" t="n">
-        <v>8.79</v>
+        <v>5.21</v>
       </c>
       <c r="H79" s="8" t="inlineStr">
         <is>
-          <t>SAHS15</t>
+          <t>SAHS</t>
         </is>
       </c>
       <c r="I79" s="9" t="inlineStr">
@@ -3376,11 +3376,11 @@
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>45928.20042824074</v>
+        <v>45929.51945601852</v>
       </c>
       <c r="B80" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6479.973588</t>
+          <t>M.15608.6481.12232</t>
         </is>
       </c>
       <c r="C80" s="3" t="inlineStr">
@@ -3399,10 +3399,10 @@
         </is>
       </c>
       <c r="F80" s="6" t="n">
-        <v>44.4</v>
+        <v>110.48</v>
       </c>
       <c r="G80" s="7" t="n">
-        <v>4.44</v>
+        <v>11.05</v>
       </c>
       <c r="H80" s="8" t="inlineStr">
         <is>
@@ -3417,11 +3417,11 @@
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>45928.19039351852</v>
+        <v>45929.51195601852</v>
       </c>
       <c r="B81" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6479.962951</t>
+          <t>M.15608.6481.9150</t>
         </is>
       </c>
       <c r="C81" s="3" t="inlineStr">
@@ -3440,10 +3440,10 @@
         </is>
       </c>
       <c r="F81" s="6" t="n">
-        <v>110.48</v>
+        <v>14.2</v>
       </c>
       <c r="G81" s="7" t="n">
-        <v>11.05</v>
+        <v>1.42</v>
       </c>
       <c r="H81" s="8" t="inlineStr">
         <is>
@@ -3458,11 +3458,11 @@
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>45928.136921296296</v>
+        <v>45929.06377314815</v>
       </c>
       <c r="B82" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6479.889929</t>
+          <t>M.15608.6480.786055</t>
         </is>
       </c>
       <c r="C82" s="3" t="inlineStr">
@@ -3481,14 +3481,14 @@
         </is>
       </c>
       <c r="F82" s="6" t="n">
-        <v>61.55</v>
+        <v>52.15</v>
       </c>
       <c r="G82" s="7" t="n">
-        <v>6.16</v>
+        <v>5.22</v>
       </c>
       <c r="H82" s="8" t="inlineStr">
         <is>
-          <t>SAHS</t>
+          <t>SAHS15</t>
         </is>
       </c>
       <c r="I82" s="9" t="inlineStr">
@@ -3499,11 +3499,11 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>45928.042291666665</v>
+        <v>45929.05862268519</v>
       </c>
       <c r="B83" s="2" t="inlineStr">
         <is>
-          <t>M.15608.6479.742586</t>
+          <t>M.15608.6480.778925</t>
         </is>
       </c>
       <c r="C83" s="3" t="inlineStr">
@@ -3522,10 +3522,10 @@
         </is>
       </c>
       <c r="F83" s="6" t="n">
-        <v>62.95</v>
+        <v>56.82</v>
       </c>
       <c r="G83" s="7" t="n">
-        <v>6.3</v>
+        <v>5.68</v>
       </c>
       <c r="H83" s="8" t="inlineStr">
         <is>
@@ -3539,84 +3539,43 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="1" t="n">
-        <v>45928.013240740744</v>
-      </c>
-      <c r="B84" s="2" t="inlineStr">
-        <is>
-          <t>M.15608.6479.683840</t>
-        </is>
-      </c>
-      <c r="C84" s="3" t="inlineStr">
-        <is>
-          <t>Airalo - The World's First eSIM Store</t>
-        </is>
-      </c>
-      <c r="D84" s="4" t="inlineStr">
-        <is>
-          <t>Sale (iOS App)</t>
-        </is>
-      </c>
-      <c r="E84" s="5" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="F84" s="6" t="n">
-        <v>47.35</v>
-      </c>
-      <c r="G84" s="7" t="n">
-        <v>4.73</v>
-      </c>
-      <c r="H84" s="8" t="inlineStr">
-        <is>
-          <t>SAHS</t>
-        </is>
-      </c>
-      <c r="I84" s="9" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" s="11" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="B85" s="12" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="C85" s="13" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="D85" s="14" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="E85" s="15" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="F85" s="16" t="n">
-        <v>4798.76</v>
-      </c>
-      <c r="G85" s="17" t="n">
-        <v>479.86</v>
-      </c>
-      <c r="H85" s="18" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="I85" s="19" t="inlineStr">
+      <c r="A84" s="11" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B84" s="12" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="C84" s="13" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="D84" s="14" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="E84" s="15" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="F84" s="16" t="n">
+        <v>4740.73</v>
+      </c>
+      <c r="G84" s="17" t="n">
+        <v>474.05</v>
+      </c>
+      <c r="H84" s="18" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="I84" s="19" t="inlineStr">
         <is>
           <t/>
         </is>

</xml_diff>